<commit_message>
LTC3: More BOM work, mostly on the LTC proper.
Plus a few minor tweaks to the charge controller and cell protection
BOMs that should not impact PCB layout.

Nearly finished with LTC BOM.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="245">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -361,6 +361,9 @@
     <t xml:space="preserve">OFFBOARD; mates to P3</t>
   </si>
   <si>
+    <t xml:space="preserve">43025-0200</t>
+  </si>
+  <si>
     <t xml:space="preserve">P6</t>
   </si>
   <si>
@@ -370,6 +373,9 @@
     <t xml:space="preserve">OFFBOARD; mates to P4</t>
   </si>
   <si>
+    <t xml:space="preserve">XHP-8</t>
+  </si>
+  <si>
     <t xml:space="preserve">P7</t>
   </si>
   <si>
@@ -395,6 +401,9 @@
   </si>
   <si>
     <t xml:space="preserve">OFFBOARD; mates to P11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XHP-2</t>
   </si>
   <si>
     <t xml:space="preserve">P11</t>
@@ -856,7 +865,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -869,15 +878,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -968,21 +973,21 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="47:47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.82995951417"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.9919028340081"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.3481781376518"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.668016194332"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1747,25 +1752,25 @@
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="3" t="s">
+      <c r="H27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1827,708 +1832,708 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="I30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="s">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="G32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="4" t="s">
+      <c r="H32" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="s">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="4" t="s">
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="I33" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="4" t="s">
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="4" t="s">
+      <c r="F34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="G34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H34" s="4" t="s">
+      <c r="H34" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="35" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="s">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="4" t="s">
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="36" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F36" s="4" t="s">
+      <c r="F36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="G36" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H36" s="4" t="s">
+      <c r="H36" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I36" s="4" t="s">
+      <c r="I36" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="4" t="s">
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="I37" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="38" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+    <row r="38" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="5" t="s">
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F39" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="G39" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="4" t="s">
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="40" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="4" t="s">
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E40" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F40" s="4" t="s">
+      <c r="F40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="G40" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="4" t="s">
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="I40" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+    <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="C41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="5" t="s">
+      <c r="F42" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="I42" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="5" t="s">
+      <c r="C46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="5" t="s">
+      <c r="F46" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="4" t="s">
+      <c r="I46" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" s="4" t="s">
+      <c r="C47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="G45" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="4" t="s">
+      <c r="F47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I45" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="46" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F48" s="4" t="s">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="C48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="F48" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
+      <c r="G48" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G49" s="4" t="s">
+      <c r="H48" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="H49" s="4" t="s">
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I49" s="4" t="s">
+      <c r="F49" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="50" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
+      <c r="G49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H49" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="I49" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F50" s="4" t="s">
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I50" s="4" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="51" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="52" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H52" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="53" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E53" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="F53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2537,56 +2542,56 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="H55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2595,56 +2600,56 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="57" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>151</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -2653,27 +2658,27 @@
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
@@ -2682,27 +2687,27 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2710,28 +2715,28 @@
       <c r="D60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>169</v>
+      <c r="E60" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2740,27 +2745,27 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2769,53 +2774,53 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -2824,27 +2829,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2853,27 +2858,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2882,259 +2887,259 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="G70" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3143,56 +3148,56 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
@@ -3201,143 +3206,143 @@
         <v>11</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E78" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>150</v>
+      <c r="E78" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>210</v>
+      <c r="C79" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E79" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>150</v>
+      <c r="E79" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C80" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>210</v>
-      </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E80" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>150</v>
+      <c r="E80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>210</v>
+        <v>217</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>213</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E81" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>150</v>
+      <c r="E81" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3346,56 +3351,56 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -3416,15 +3421,15 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3445,15 +3450,15 @@
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3474,44 +3479,44 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3532,15 +3537,15 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -3561,15 +3566,15 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
@@ -3590,7 +3595,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: LTC schematic changes; LTC BOM work.
* Replaced LTC external power and trigger circuits' off-board manual
  override switches with board-mounted tactile momentary switches.
  Simplifies assembly, and should be more than adequate for debugging
  purposes.

* Changed cell protection diodes D1 and D6 from Rohm 1SS355 to ComChip
  CDSU4148.  CDSU4148 is already used on the LTC board, and is higher
  spec than the 1SS355.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="243">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -220,22 +220,16 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">1SS355</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1SS355TE-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Standard 80V 100mA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/semiconductors/Rohm-1SS355-Switching_Diode.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diodes_SMD:TUMD2</t>
+    <t xml:space="preserve">CDSU4148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard 75V 150mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodes_SMD:SOD-523</t>
   </si>
   <si>
     <t xml:space="preserve">D2</t>
@@ -865,7 +859,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -878,11 +872,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -973,21 +971,21 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.4534412955466"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.9919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -1836,675 +1834,675 @@
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="H30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
+      <c r="G32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="H33" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="I33" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F34" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="F35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="H35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="1" t="s">
+      <c r="G36" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="I36" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="G37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="1" t="s">
+      <c r="I37" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="G37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="1" t="s">
+    </row>
+    <row r="38" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I37" s="1" t="s">
+      <c r="B38" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="38" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+      <c r="C38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="G39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I39" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="G40" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E40" s="1" t="s">
+      <c r="F42" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F40" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I42" s="4" t="s">
+      <c r="I42" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I44" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B45" s="1" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E45" s="1" t="s">
+      <c r="F46" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="I46" s="4" t="s">
+      <c r="I46" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B47" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="I47" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" s="1" t="s">
+      <c r="G48" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="H48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="I48" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="1" t="s">
+      <c r="G49" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="H49" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="I49" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="F50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" s="1" t="s">
+      <c r="H50" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G50" s="1" t="s">
+      <c r="I50" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="1" t="s">
+      <c r="G52" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="F52" s="1" t="s">
+      <c r="H52" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2513,16 +2511,16 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F53" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H53" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>10</v>
@@ -2530,297 +2528,297 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="F54" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="1" t="s">
+      <c r="G54" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F54" s="1" t="s">
+      <c r="H54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I54" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H54" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I54" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
+      <c r="G55" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="G56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="B57" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="C57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>154</v>
+      <c r="E57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E58" s="1" t="s">
+      <c r="G58" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F58" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E59" s="1" t="s">
+      <c r="G59" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G59" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F60" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="1" t="s">
+      <c r="G60" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F60" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F61" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" s="1" t="s">
+      <c r="G61" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E62" s="1" t="s">
+      <c r="G62" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F62" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G62" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="F63" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="G63" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F63" s="1" t="s">
+      <c r="H63" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I63" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -2829,27 +2827,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G64" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F64" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2858,27 +2856,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2887,578 +2885,578 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G66" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="D67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F67" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E67" s="1" t="s">
+      <c r="G67" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="1" t="s">
+      <c r="G68" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F69" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F69" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
+      <c r="G70" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F71" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E71" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E72" s="1" t="s">
+      <c r="G72" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F72" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="1" t="s">
+      <c r="G73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F73" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F74" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E74" s="1" t="s">
+      <c r="G74" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F74" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E75" s="1" t="s">
+      <c r="G75" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F75" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="D76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F76" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="C76" s="1" t="s">
+      <c r="G76" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I76" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I76" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F77" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="1" t="s">
+      <c r="G77" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F77" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C78" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="D78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C78" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E78" s="1" t="s">
+      <c r="G78" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="1" t="s">
+      <c r="G79" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E80" s="1" t="s">
+      <c r="G80" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F80" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>213</v>
+        <v>215</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>211</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="1" t="s">
+      <c r="G82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="I82" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="I82" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="D83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="1" t="s">
+      <c r="G83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="F83" s="1" t="s">
+      <c r="I83" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I85" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3479,15 +3477,15 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3508,15 +3506,15 @@
         <v>10</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3537,15 +3535,15 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -3566,15 +3564,15 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
@@ -3595,7 +3593,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Minor changes to Cell Protection BOM.
Nothing that impacts PCB layout.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="251">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -301,7 +301,10 @@
     <t xml:space="preserve">B2B-XH-A(LF)(SN)</t>
   </si>
   <si>
-    <t xml:space="preserve">http://www.jst-mfg.com/product/pdf/eng/eXH.pdf</t>
+    <t xml:space="preserve">2 pos vertical header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/JST-XH-2.5mm_pitch_Disconnectable_Crimp_style_connectors.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Connectors_JST:JST_XH_B02B-XH-A_08x2.50mm_Straight</t>
@@ -331,6 +334,9 @@
     <t xml:space="preserve">43045-0228</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x01_Straight_43045-0228</t>
   </si>
   <si>
@@ -343,6 +349,9 @@
     <t xml:space="preserve">B8B-XH-A(LF)(SN)</t>
   </si>
   <si>
+    <t xml:space="preserve">8 pos vertical header</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connectors_JST:JST_XH_B08B-XH-A_08x2.50mm_Straight</t>
   </si>
   <si>
@@ -358,6 +367,12 @@
     <t xml:space="preserve">43025-0200</t>
   </si>
   <si>
+    <t xml:space="preserve">2 pos connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-Micro_Fit_3_Family.pdf</t>
+  </si>
+  <si>
     <t xml:space="preserve">P6</t>
   </si>
   <si>
@@ -370,6 +385,9 @@
     <t xml:space="preserve">XHP-8</t>
   </si>
   <si>
+    <t xml:space="preserve">8 pos connector</t>
+  </si>
+  <si>
     <t xml:space="preserve">P7</t>
   </si>
   <si>
@@ -388,6 +406,9 @@
     <t xml:space="preserve">B4B-XH-A(LF)(SN)</t>
   </si>
   <si>
+    <t xml:space="preserve">4 pos vertical header</t>
+  </si>
+  <si>
     <t xml:space="preserve">Connectors_JST:JST_XH_B04B-XH-A_02x2.50mm_Straight</t>
   </si>
   <si>
@@ -401,6 +422,9 @@
   </si>
   <si>
     <t xml:space="preserve">P11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to batt temp sense</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
@@ -971,22 +995,22 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.0323886639676"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="44.9919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.8825910931174"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.6428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.1887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2053,26 +2077,26 @@
         <v>92</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="H37" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I37" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="4" t="s">
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="4" t="s">
+      <c r="B38" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -2081,48 +2105,48 @@
       <c r="F38" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>97</v>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>89</v>
@@ -2131,48 +2155,48 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>93</v>
+        <v>109</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>93</v>
+        <v>115</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2180,28 +2204,28 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>93</v>
+        <v>121</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>10</v>
@@ -2209,65 +2233,65 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>89</v>
@@ -2276,48 +2300,48 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>93</v>
+        <v>128</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>93</v>
+        <v>115</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>94</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>10</v>
@@ -2325,7 +2349,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>89</v>
@@ -2334,7 +2358,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>91</v>
@@ -2343,21 +2367,21 @@
         <v>92</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H47" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="H47" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="I47" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -2366,27 +2390,27 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>11</v>
@@ -2395,27 +2419,27 @@
         <v>11</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -2424,56 +2448,56 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I51" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
@@ -2482,27 +2506,27 @@
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2511,16 +2535,16 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>10</v>
@@ -2528,10 +2552,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2540,27 +2564,27 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>11</v>
@@ -2569,85 +2593,85 @@
         <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>149</v>
-      </c>
       <c r="F56" s="1" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="6" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -2656,27 +2680,27 @@
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
@@ -2685,27 +2709,27 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2714,27 +2738,27 @@
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2743,27 +2767,27 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2772,82 +2796,82 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F64" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="G64" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2856,27 +2880,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2885,259 +2909,259 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>188</v>
-      </c>
       <c r="C73" s="1" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3146,56 +3170,56 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
@@ -3204,143 +3228,143 @@
         <v>11</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3349,56 +3373,56 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -3419,15 +3443,15 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3448,15 +3472,15 @@
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3477,15 +3501,15 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3506,15 +3530,15 @@
         <v>10</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3535,44 +3559,44 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
@@ -3593,7 +3617,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Modified Cell Protection schematic, correcting R4 value.
No impact to PCB layout.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="252">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -313,7 +313,10 @@
     <t xml:space="preserve">P2</t>
   </si>
   <si>
-    <t xml:space="preserve">PIN_HEAD_1x2</t>
+    <t xml:space="preserve">pin header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x2 pin header</t>
   </si>
   <si>
     <t xml:space="preserve">Pin_Headers:Pin_Header_Straight_1x02</t>
@@ -526,10 +529,10 @@
     <t xml:space="preserve">R4</t>
   </si>
   <si>
-    <t xml:space="preserve">6.89k</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNAVAILABLE</t>
+    <t xml:space="preserve">6.98k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0805FR-076K98L</t>
   </si>
   <si>
     <t xml:space="preserve">R5</t>
@@ -783,7 +786,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -821,8 +824,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,12 +842,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
-        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -883,7 +886,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -900,15 +903,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -925,66 +924,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF9999"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -995,22 +934,22 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H43" activeCellId="0" sqref="H43"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.6428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="53.1887755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="52.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2079,7 +2018,7 @@
       <c r="G37" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="4" t="s">
+      <c r="H37" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -2099,54 +2038,54 @@
       <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="5" t="s">
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>89</v>
@@ -2155,48 +2094,48 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H40" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H41" s="4" t="s">
         <v>116</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2204,27 +2143,27 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H42" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -2233,65 +2172,65 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>93</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>89</v>
@@ -2300,47 +2239,47 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="H45" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H45" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H46" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -2349,7 +2288,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>89</v>
@@ -2358,7 +2297,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>91</v>
@@ -2369,7 +2308,7 @@
       <c r="G47" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H47" s="4" t="s">
+      <c r="H47" s="1" t="s">
         <v>94</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -2378,10 +2317,10 @@
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -2390,56 +2329,56 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -2448,27 +2387,27 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
@@ -2477,27 +2416,27 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
@@ -2506,27 +2445,27 @@
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2535,16 +2474,16 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>10</v>
@@ -2552,10 +2491,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2564,56 +2503,56 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2622,56 +2561,56 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="57" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>160</v>
+      <c r="H57" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -2680,27 +2619,27 @@
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
@@ -2709,27 +2648,27 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2738,27 +2677,27 @@
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2767,27 +2706,27 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2796,53 +2735,53 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -2851,27 +2790,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2880,27 +2819,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2909,259 +2848,259 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="G68" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3170,56 +3109,56 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G76" s="1" t="s">
-        <v>211</v>
-      </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
@@ -3228,143 +3167,143 @@
         <v>11</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C78" s="7" t="s">
         <v>219</v>
       </c>
+      <c r="C78" s="6" t="s">
+        <v>220</v>
+      </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="G79" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>219</v>
+        <v>224</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>220</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>224</v>
-      </c>
       <c r="G81" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3373,56 +3312,56 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -3443,15 +3382,15 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3472,15 +3411,15 @@
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3501,15 +3440,15 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3530,15 +3469,15 @@
         <v>10</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3559,15 +3498,15 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -3588,15 +3527,15 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
@@ -3617,7 +3556,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Cleaned up datasheet collection.
Also updated datasheet URLs in schematics and BOM spreadsheets.  No
impact to PCB layout.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="253">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t xml:space="preserve">Standard 75V 150mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/semiconductors/ComChip-CDSU4148-SMD_Switching_Diode.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes_SMD:SOD-523</t>
@@ -935,21 +938,21 @@
   <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+      <selection pane="topLeft" activeCell="H54" activeCellId="0" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1816,18 +1819,18 @@
         <v>68</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
@@ -1836,56 +1839,56 @@
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>11</v>
@@ -1894,27 +1897,27 @@
         <v>11</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>11</v>
@@ -1923,24 +1926,24 @@
         <v>11</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>66</v>
@@ -1961,18 +1964,18 @@
         <v>68</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>11</v>
@@ -1981,56 +1984,56 @@
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>11</v>
@@ -2045,97 +2048,97 @@
         <v>11</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2143,28 +2146,28 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>10</v>
@@ -2172,115 +2175,115 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>10</v>
@@ -2288,39 +2291,39 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -2329,56 +2332,56 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="I49" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -2387,27 +2390,27 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F50" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="G50" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
@@ -2416,27 +2419,27 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
@@ -2445,27 +2448,27 @@
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2474,16 +2477,16 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>10</v>
@@ -2491,10 +2494,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2503,56 +2506,56 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2561,27 +2564,27 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>11</v>
@@ -2590,27 +2593,27 @@
         <v>11</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>10</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -2619,27 +2622,27 @@
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
@@ -2648,27 +2651,27 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2677,27 +2680,27 @@
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2706,27 +2709,27 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2735,53 +2738,53 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -2790,27 +2793,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2819,27 +2822,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2848,259 +2851,259 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F68" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="G68" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3109,56 +3112,56 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F76" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G76" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="G76" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
@@ -3167,143 +3170,143 @@
         <v>11</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="G79" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="B81" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>225</v>
-      </c>
       <c r="G81" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3312,56 +3315,56 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -3382,15 +3385,15 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>11</v>
@@ -3411,15 +3414,15 @@
         <v>10</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>11</v>
@@ -3440,15 +3443,15 @@
         <v>10</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>11</v>
@@ -3469,15 +3472,15 @@
         <v>10</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>11</v>
@@ -3498,15 +3501,15 @@
         <v>10</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>11</v>
@@ -3527,15 +3530,15 @@
         <v>10</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>11</v>
@@ -3556,7 +3559,7 @@
         <v>10</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LTC3: Updated BOM info for recently changed Cell Prot. DC connectors.
</commit_message>
<xml_diff>
--- a/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
+++ b/ltc3/bom/cell_protection/LTC3_Cell_Protection.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="256">
   <si>
     <t xml:space="preserve">Refs</t>
   </si>
@@ -331,19 +331,22 @@
     <t xml:space="preserve">MicroFit header</t>
   </si>
   <si>
-    <t xml:space="preserve">CONN_BATT_MAIN</t>
+    <t xml:space="preserve">BATT_MAIN_CONN</t>
   </si>
   <si>
     <t xml:space="preserve">Molex</t>
   </si>
   <si>
-    <t xml:space="preserve">43045-0228</t>
+    <t xml:space="preserve">43045-0428</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 pos vertical header</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-43045-Micro_Fit_3_dual_row_vertical_through_hole_header.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x01_Straight_43045-0228</t>
+    <t xml:space="preserve">Connectors_Molex:Molex_Microfit3_Header_02x02_Straight_43045-0428</t>
   </si>
   <si>
     <t xml:space="preserve">P4</t>
@@ -370,67 +373,73 @@
     <t xml:space="preserve">OFFBOARD; mates to P3</t>
   </si>
   <si>
-    <t xml:space="preserve">43025-0200</t>
+    <t xml:space="preserve">43025-0400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 pos connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-Micro_Fit_3_Family.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XH connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFBOARD; mates to P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XHP-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 pos connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC_IN_OUT (to LTC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DC_IN_OUT (to Charge Cont.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to LTC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B4B-XH-A(LF)(SN)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors_JST:JST_XH_B04B-XH-A_02x2.50mm_Straight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFFBOARD; mates to P11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XHP-2</t>
   </si>
   <si>
     <t xml:space="preserve">2 pos connector</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/psas/launch-tower/blob/master/ltc3/doc/datasheets/connectors/Molex-Micro_Fit_3_Family.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XH connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OFFBOARD; mates to P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XHP-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8 pos connector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to Charge Controller</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">to LTC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B4B-XH-A(LF)(SN)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4 pos vertical header</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connectors_JST:JST_XH_B04B-XH-A_02x2.50mm_Straight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OFFBOARD; mates to P11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XHP-2</t>
-  </si>
-  <si>
     <t xml:space="preserve">P11</t>
   </si>
   <si>
     <t xml:space="preserve">to batt temp sense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connectors_JST:JST_EH_B02B-EH-A_02x2.50mm_Straight</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
@@ -889,7 +898,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -899,10 +908,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -937,22 +942,22 @@
   </sheetPr>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H54" activeCellId="0" sqref="H54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G42" activeCellId="0" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="51.969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="36.719387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="50.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="1" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1800,28 +1805,28 @@
       <c r="A30" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H30" s="3" t="s">
+      <c r="H30" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1945,28 +1950,28 @@
       <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="H35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="1" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2041,10 +2046,10 @@
       <c r="D38" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F38" s="4" t="s">
+      <c r="E38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G38" s="1" t="s">
@@ -2077,18 +2082,18 @@
         <v>105</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>90</v>
@@ -2097,48 +2102,48 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>104</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>10</v>
@@ -2146,25 +2151,25 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>95</v>
@@ -2175,7 +2180,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>102</v>
@@ -2184,7 +2189,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>104</v>
@@ -2193,18 +2198,18 @@
         <v>105</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>102</v>
@@ -2213,7 +2218,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>104</v>
@@ -2222,18 +2227,18 @@
         <v>105</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>90</v>
@@ -2242,45 +2247,45 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>95</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>95</v>
@@ -2291,7 +2296,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>90</v>
@@ -2300,7 +2305,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>92</v>
@@ -2315,15 +2320,15 @@
         <v>95</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>11</v>
@@ -2332,56 +2337,56 @@
         <v>11</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
@@ -2390,27 +2395,27 @@
         <v>11</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
@@ -2419,27 +2424,27 @@
         <v>11</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>11</v>
@@ -2448,27 +2453,27 @@
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>11</v>
@@ -2477,16 +2482,16 @@
         <v>12</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>10</v>
@@ -2494,10 +2499,10 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>11</v>
@@ -2506,56 +2511,56 @@
         <v>11</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G55" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F55" s="1" t="s">
+      <c r="H55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I55" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>11</v>
@@ -2564,56 +2569,56 @@
         <v>11</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I56" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="57" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>162</v>
+      <c r="F57" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>11</v>
@@ -2622,27 +2627,27 @@
         <v>11</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>11</v>
@@ -2651,27 +2656,27 @@
         <v>11</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>11</v>
@@ -2680,27 +2685,27 @@
         <v>11</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>11</v>
@@ -2709,27 +2714,27 @@
         <v>11</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>11</v>
@@ -2738,53 +2743,53 @@
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>11</v>
@@ -2793,27 +2798,27 @@
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>11</v>
@@ -2822,27 +2827,27 @@
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>11</v>
@@ -2851,259 +2856,259 @@
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>198</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="D69" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="G70" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H71" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>11</v>
@@ -3112,56 +3117,56 @@
         <v>11</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>11</v>
@@ -3170,143 +3175,143 @@
         <v>11</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>221</v>
+        <v>223</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>221</v>
+      <c r="C79" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C80" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>221</v>
-      </c>
       <c r="D80" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>221</v>
+        <v>228</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>224</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>11</v>
@@ -3315,56 +3320,56 @@
         <v>11</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>11</v>
@@ -3385,181 +3390,181 @@
         <v>10</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="1" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I88" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I85" s="1" t="s">
+      <c r="C89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="B86" s="1" t="s">
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I87" s="1" t="s">
+      <c r="C90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>